<commit_message>
Updated files to not include extra sheets or data
</commit_message>
<xml_diff>
--- a/ExcelFiles/WGUPS Distance Table.xlsx
+++ b/ExcelFiles/WGUPS Distance Table.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/specter/PycharmProjects/C950/ExcelFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a165164663ef0029/Documents/GitHub/DS2-C950/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57384A4F-4BF0-F64D-A038-170067B83678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{57384A4F-4BF0-F64D-A038-170067B83678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C84BFC14-96E9-4339-83F3-105CA7097C4C}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="500" windowWidth="24680" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$7:$AC$35</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -695,6 +698,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -958,26 +965,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:W5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" style="2" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="29" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="29" width="5.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -989,7 +999,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -1001,7 +1011,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -1013,7 +1023,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="23" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1049,7 @@
       <c r="V4" s="24"/>
       <c r="W4" s="24"/>
     </row>
-    <row r="5" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -1063,7 +1073,7 @@
       <c r="V5" s="24"/>
       <c r="W5" s="24"/>
     </row>
-    <row r="6" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="25" t="s">
         <v>1</v>
       </c>
@@ -1082,7 +1092,7 @@
       <c r="P6" s="24"/>
       <c r="Q6" s="24"/>
     </row>
-    <row r="7" spans="1:29" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1111,7 +1121,7 @@
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
     </row>
-    <row r="8" spans="1:29" ht="166" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="160.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="13" t="s">
         <v>56</v>
       </c>
@@ -1198,7 +1208,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="52" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="48" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1297,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>4</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>6</v>
       </c>
@@ -1465,7 +1475,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="36" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>8</v>
       </c>
@@ -1554,7 +1564,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="36" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>10</v>
       </c>
@@ -1643,7 +1653,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="36" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>12</v>
       </c>
@@ -1732,7 +1742,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="36" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>14</v>
       </c>
@@ -1821,7 +1831,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>16</v>
       </c>
@@ -1910,7 +1920,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>18</v>
       </c>
@@ -1999,7 +2009,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>20</v>
       </c>
@@ -2088,7 +2098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>22</v>
       </c>
@@ -2177,7 +2187,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>24</v>
       </c>
@@ -2266,7 +2276,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>26</v>
       </c>
@@ -2355,7 +2365,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>28</v>
       </c>
@@ -2444,7 +2454,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>30</v>
       </c>
@@ -2533,7 +2543,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
         <v>32</v>
       </c>
@@ -2622,7 +2632,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" ht="36" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>57</v>
       </c>
@@ -2711,7 +2721,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="39" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" ht="36" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
         <v>36</v>
       </c>
@@ -2800,7 +2810,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="39" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="36" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
         <v>38</v>
       </c>
@@ -2889,7 +2899,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
         <v>40</v>
       </c>
@@ -2978,7 +2988,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="39" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" ht="36" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>42</v>
       </c>
@@ -3067,7 +3077,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>44</v>
       </c>
@@ -3156,7 +3166,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
         <v>46</v>
       </c>
@@ -3245,7 +3255,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="39" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" ht="36" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>48</v>
       </c>
@@ -3334,7 +3344,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" ht="23.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
         <v>50</v>
       </c>
@@ -3423,7 +3433,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" ht="24" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
         <v>52</v>
       </c>
@@ -3512,7 +3522,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="23.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" ht="23.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="19" t="s">
         <v>54</v>
       </c>
@@ -3608,12 +3618,49 @@
     <mergeCell ref="C6:Q6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Performance_x0020_Steps_x0020_Completed>
+    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>N/A</Value>
+    </Step_x0020_Completed>
+    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <Value>Objective</Value>
+    </Assessment_x0020_Type>
+    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Editor0>
+    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C39F2A75005F2D43B30369DAED2CCB1C" ma:contentTypeVersion="40" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="67abd11da167d8eab610c259a823e4c7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xmlns:ns3="1f707338-ea0f-4fe5-baee-59b996692b22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d3ab84303ed41503c975572ff37e680" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4051,7 +4098,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4060,44 +4107,26 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Vendor xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">N/A</Vendor>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Launch_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Discipline xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_code xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Performance_x0020_Steps_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Performance_x0020_Steps_x0020_Completed>
-    <Course_x0020_short_x0020_name xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Course_x0020_number xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Course_x0020_title xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <d5fh xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Step_x0020_Completed xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>N/A</Value>
-    </Step_x0020_Completed>
-    <Assessment_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <Value>Objective</Value>
-    </Assessment_x0020_Type>
-    <Publication_x0020_Date xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <SME xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-    <Editor0 xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Editor0>
-    <Doc_x0020_Type xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <qrac xmlns="0feec74c-ecc7-44c3-9c64-3623cf89ed41" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="e7b1d905-24de-49f1-ac69-282527225b8e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="986a1e7c-3408-4565-abd6-87412778acff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83388E46-74FF-49C2-B8E6-3BEB0ECD2207}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4117,29 +4146,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="e7b1d905-24de-49f1-ac69-282527225b8e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="986a1e7c-3408-4565-abd6-87412778acff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="0feec74c-ecc7-44c3-9c64-3623cf89ed41"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>